<commit_message>
Lab 2 Part 1 finished.
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>NUMTASKS</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Part 1 ISR execution time</t>
+  </si>
+  <si>
+    <t>Part 1 Event Latency</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>Time (us) Lower</t>
   </si>
 </sst>
 </file>
@@ -603,7 +612,585 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>The relation between PRIORITY and the event delay.</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-NL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (us)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$24:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ED45-4C61-9904-A101AD674662}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (us) Lower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$24:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$24:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ED45-4C61-9904-A101AD674662}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2062254928"/>
+        <c:axId val="275388896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2062254928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>PRIORITY</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="275388896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="275388896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Event Delay (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062254928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1146,6 +1733,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1184,6 +2287,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193D0087-FD34-4928-A138-E063961926EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1193,6 +2332,18 @@
   <tableColumns count="2">
     <tableColumn id="1" name="NUMTASKS"/>
     <tableColumn id="2" name="Time (us)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A23:C28" totalsRowShown="0">
+  <autoFilter ref="A23:C28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="PRIORITY"/>
+    <tableColumn id="2" name="Time (us)"/>
+    <tableColumn id="3" name="Time (us) Lower"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1495,16 +2646,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1633,20 +2785,95 @@
         <v>942</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
       <c r="B17">
         <v>980</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>261</v>
+      </c>
+      <c r="C24">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>224</v>
+      </c>
+      <c r="C25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>187</v>
+      </c>
+      <c r="C26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>149</v>
+      </c>
+      <c r="C27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>112</v>
+      </c>
+      <c r="C28">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>